<commit_message>
updates w/ ram comments
</commit_message>
<xml_diff>
--- a/Olympic Athletes/hockey.xlsx
+++ b/Olympic Athletes/hockey.xlsx
@@ -15,11 +15,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="timecalc" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1825" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="511">
   <si>
     <t>name</t>
   </si>
@@ -1536,6 +1537,33 @@
   </si>
   <si>
     <t>distance travelled in 11.08 strides</t>
+  </si>
+  <si>
+    <t>distance travelled in 1 stride (m)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assumption </t>
+  </si>
+  <si>
+    <t>no of strides per sec</t>
+  </si>
+  <si>
+    <t>Distance covered in 1 sec(m)</t>
+  </si>
+  <si>
+    <t>4.968 m</t>
+  </si>
+  <si>
+    <t>1 sec</t>
+  </si>
+  <si>
+    <t>1 m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 m is covered in(s) </t>
+  </si>
+  <si>
+    <t>27.5 m is covered in(s)</t>
   </si>
 </sst>
 </file>
@@ -22434,13 +22462,14 @@
   <dimension ref="A1:V28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="J3" sqref="J3:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -22519,10 +22548,10 @@
         <v>300</v>
       </c>
       <c r="J2">
-        <v>547.89712343688052</v>
+        <v>550</v>
       </c>
       <c r="K2">
-        <v>305.08211670077372</v>
+        <v>300</v>
       </c>
       <c r="L2" t="s">
         <v>478</v>
@@ -22569,13 +22598,13 @@
         <v>625</v>
       </c>
       <c r="I3">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="J3">
-        <v>546.03410925962544</v>
+        <v>550</v>
       </c>
       <c r="K3">
-        <v>303.96941790747411</v>
+        <v>300</v>
       </c>
       <c r="L3" t="s">
         <v>479</v>
@@ -22625,10 +22654,10 @@
         <v>310</v>
       </c>
       <c r="J4">
-        <v>543.45725987381422</v>
+        <v>550</v>
       </c>
       <c r="K4">
-        <v>302.71406755720756</v>
+        <v>300</v>
       </c>
       <c r="L4" t="s">
         <v>480</v>
@@ -22678,10 +22707,10 @@
         <v>280</v>
       </c>
       <c r="J5">
-        <v>542.86111236372551</v>
+        <v>550</v>
       </c>
       <c r="K5">
-        <v>300.00423088788011</v>
+        <v>300</v>
       </c>
       <c r="L5" t="s">
         <v>481</v>
@@ -22728,13 +22757,13 @@
         <v>550</v>
       </c>
       <c r="I6">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="J6">
-        <v>542.4529017787662</v>
+        <v>550</v>
       </c>
       <c r="K6">
-        <v>296.87978319055577</v>
+        <v>300</v>
       </c>
       <c r="L6" t="s">
         <v>482</v>
@@ -22784,10 +22813,10 @@
         <v>300</v>
       </c>
       <c r="J7">
-        <v>543.65098258785088</v>
+        <v>550</v>
       </c>
       <c r="K7">
-        <v>293.66038254582435</v>
+        <v>300</v>
       </c>
       <c r="L7" t="s">
         <v>483</v>
@@ -22836,6 +22865,12 @@
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>498</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>499</v>
+      </c>
       <c r="C11">
         <v>0</v>
       </c>
@@ -22879,6 +22914,12 @@
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>547.89712343688052</v>
+      </c>
+      <c r="B12">
+        <v>305.08211670077372</v>
+      </c>
       <c r="C12">
         <v>1</v>
       </c>
@@ -22922,6 +22963,12 @@
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>546.03410925962544</v>
+      </c>
+      <c r="B13">
+        <v>303.96941790747411</v>
+      </c>
       <c r="C13">
         <v>2</v>
       </c>
@@ -22965,6 +23012,12 @@
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>543.45725987381422</v>
+      </c>
+      <c r="B14">
+        <v>302.71406755720756</v>
+      </c>
       <c r="C14">
         <v>3</v>
       </c>
@@ -23008,6 +23061,12 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>542.86111236372551</v>
+      </c>
+      <c r="B15">
+        <v>300.00423088788011</v>
+      </c>
       <c r="C15">
         <v>4</v>
       </c>
@@ -23051,6 +23110,12 @@
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>542.4529017787662</v>
+      </c>
+      <c r="B16">
+        <v>296.87978319055577</v>
+      </c>
       <c r="C16">
         <v>5</v>
       </c>
@@ -23093,7 +23158,13 @@
         <v>229.34172495143946</v>
       </c>
     </row>
-    <row r="17" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>543.65098258785088</v>
+      </c>
+      <c r="B17">
+        <v>293.66038254582435</v>
+      </c>
       <c r="L17">
         <f t="shared" si="4"/>
         <v>345.1704878196897</v>
@@ -23121,7 +23192,7 @@
         <v>207.64326224360173</v>
       </c>
     </row>
-    <row r="18" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
         <v>491</v>
       </c>
@@ -23132,7 +23203,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="19" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C19">
         <f>180/7</f>
         <v>25.714285714285715</v>
@@ -23144,7 +23215,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>493</v>
       </c>
@@ -23176,7 +23247,7 @@
         <v>179.99799999999999</v>
       </c>
     </row>
-    <row r="22" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F22">
         <f>550+100*COS(F20)</f>
         <v>633.5772150614473</v>
@@ -23186,7 +23257,7 @@
         <v>383.57721506144736</v>
       </c>
     </row>
-    <row r="23" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F23">
         <f t="shared" ref="F23:F28" si="10">550+100*COS(F21)</f>
         <v>650</v>
@@ -23196,7 +23267,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="24" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F24">
         <f t="shared" si="10"/>
         <v>601.95253555926161</v>
@@ -23206,7 +23277,7 @@
         <v>351.95253555926161</v>
       </c>
     </row>
-    <row r="25" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F25">
         <f t="shared" si="10"/>
         <v>454.75686446775927</v>
@@ -23216,7 +23287,7 @@
         <v>204.75686446775927</v>
       </c>
     </row>
-    <row r="26" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F26">
         <f t="shared" si="10"/>
         <v>583.11691705061617</v>
@@ -23226,7 +23297,7 @@
         <v>333.11691705061611</v>
       </c>
     </row>
-    <row r="27" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F27">
         <f t="shared" si="10"/>
         <v>478.49287506844996</v>
@@ -23236,7 +23307,7 @@
         <v>228.49287506844996</v>
       </c>
     </row>
-    <row r="28" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F28">
         <f t="shared" si="10"/>
         <v>584.42875243643891</v>
@@ -23252,6 +23323,243 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="10" t="s">
+        <v>470</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="D1" t="s">
+        <v>500</v>
+      </c>
+      <c r="E1" t="s">
+        <v>502</v>
+      </c>
+      <c r="F1" t="s">
+        <v>505</v>
+      </c>
+      <c r="G1" t="s">
+        <v>509</v>
+      </c>
+      <c r="H1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="C2" s="12">
+        <v>184</v>
+      </c>
+      <c r="D2">
+        <v>248.4</v>
+      </c>
+      <c r="E2">
+        <f>D2/100</f>
+        <v>2.484</v>
+      </c>
+      <c r="F2">
+        <f>E2*2</f>
+        <v>4.968</v>
+      </c>
+      <c r="G2">
+        <f>1/F2</f>
+        <v>0.20128824476650564</v>
+      </c>
+      <c r="H2">
+        <f>G2*27.5</f>
+        <v>5.5354267310789051</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>419</v>
+      </c>
+      <c r="C3" s="12">
+        <v>183.7777778</v>
+      </c>
+      <c r="D3">
+        <v>248.10000003000002</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E7" si="0">D3/100</f>
+        <v>2.4810000003000003</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F7" si="1">E3*2</f>
+        <v>4.9620000006000007</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G7" si="2">1/F3</f>
+        <v>0.20153164044318439</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H7" si="3">G3*27.5</f>
+        <v>5.5421201121875709</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="C4" s="12">
+        <v>180.83333329999999</v>
+      </c>
+      <c r="D4">
+        <v>244.12499995499999</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>2.4412499995500001</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>4.8824999991000002</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>0.20481310807666805</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="3"/>
+        <v>5.6323604721083713</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="12">
+        <v>180.7222222</v>
+      </c>
+      <c r="D5">
+        <v>243.97499997000003</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>2.4397499997000001</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>4.8794999994000001</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>0.20493903066358507</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="3"/>
+        <v>5.6358233432485898</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="C6" s="12">
+        <v>178.66666670000001</v>
+      </c>
+      <c r="D6">
+        <v>241.20000004500002</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>2.4120000004500004</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>4.8240000009000008</v>
+      </c>
+      <c r="G6">
+        <f>1/F6</f>
+        <v>0.20729684904921905</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="3"/>
+        <v>5.7006633488535243</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="12">
+        <v>177.05555559999999</v>
+      </c>
+      <c r="D7">
+        <v>239.02500006</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>2.3902500006</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>4.7805000012000001</v>
+      </c>
+      <c r="G7">
+        <f>1/F7</f>
+        <v>0.20918313978641986</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="3"/>
+        <v>5.752536344126546</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>504</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>506</v>
+      </c>
+      <c r="G14" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>508</v>
+      </c>
+      <c r="G15">
+        <f>1/4.968</f>
+        <v>0.20128824476650564</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>

</xml_diff>